<commit_message>
optimization library 0.4.0 with arrays
</commit_message>
<xml_diff>
--- a/additional files/inputOptimization.xlsx
+++ b/additional files/inputOptimization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Noorjax Dropbox\felipe haro\00 - current\Noorjax Library\Generic Monte-Carlo Library\07 - Optimization Library\optimizationWithMontecarlo\additional files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohei\Noorjax Dropbox\Soheila Antar\Generic Monte-Carlo Library\00 - Models\02 - McOptCombined\optimWithMC3.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9E43BC-98B1-4A07-9AB3-FE35FB93CA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E90DF7-33D3-4E73-B575-01F455525253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2650" yWindow="2110" windowWidth="15210" windowHeight="9170" xr2:uid="{A171BDC2-95BE-4336-9B5E-292EF29FBC2F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A171BDC2-95BE-4336-9B5E-292EF29FBC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="params_ranges" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="29">
   <si>
     <t>parameter</t>
   </si>
@@ -68,12 +68,70 @@
   </si>
   <si>
     <t>bound</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>p2*p3</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>variable-variable1</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>is an array</t>
+  </si>
+  <si>
+    <t>array size</t>
+  </si>
+  <si>
+    <t>p1Array</t>
+  </si>
+  <si>
+    <t>p7</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>CONTINUOUS</t>
+  </si>
+  <si>
+    <t>DISCRETE</t>
+  </si>
+  <si>
+    <t>on array</t>
+  </si>
+  <si>
+    <t>2*p1Array[0]+p1Array[2]/2</t>
+  </si>
+  <si>
+    <t>p6+p7</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,9 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,46 +507,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010575B9-F756-4818-BDE4-3317344B56F0}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="12.21875"/>
+    <col min="4" max="4" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s" s="0">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{9BE801CA-7526-4DED-B71D-A2188E613ACD}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{1F3D22C8-60CC-4EA1-8470-2D3E2FAB60B2}">
       <formula1>"CONTINUOUS, DISCRETE, FIXED, BOOLEAN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{F4DCDA35-49B4-4B2C-9D0D-157075A7E68F}">
+      <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -494,37 +695,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533F1823-82DC-4534-8350-D37916D32DEF}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="A2:E3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875"/>
+    <col min="2" max="3" customWidth="true" width="13.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576 C2:C1048576" xr:uid="{BB0538A1-A811-4C5C-9229-5E9E07B26106}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -533,36 +802,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BE615E-0897-4568-8DE6-9A70984B89E6}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D2" s="1"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{F8A07CD2-69CF-45D3-B543-AB4C9B3AD210}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>